<commit_message>
Initial commit of owain-guideline-table
</commit_message>
<xml_diff>
--- a/data/Owain-Guidelines-table.xlsx
+++ b/data/Owain-Guidelines-table.xlsx
@@ -236,9 +236,6 @@
     <t>Practice Guide</t>
   </si>
   <si>
-    <t>Better Infrastructure Decision Making: Guidelines for Making Submissions to Infrastructure Australia’s Infrastructure Planning Process</t>
-  </si>
-  <si>
     <t>Business Case Template</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t>Guideline</t>
+  </si>
+  <si>
+    <t>Better Infrastructure Decision Making: Guidelines for Making Submissions to Infrastructure Australia's Infrastructure Planning Process</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,13 +689,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
         <v>25</v>
@@ -1190,62 +1190,62 @@
         <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
         <v>20</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
         <v>20</v>
       </c>
       <c r="C55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,29 +1256,29 @@
         <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
         <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1289,29 +1289,29 @@
         <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
         <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1322,18 +1322,18 @@
         <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>